<commit_message>
new release [bulk selection added]
</commit_message>
<xml_diff>
--- a/data/db/employes.xlsx
+++ b/data/db/employes.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L178"/>
+  <dimension ref="A1:M178"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -442,6 +442,9 @@
       <c r="L1" t="str">
         <v>LAST_UPDATED_YEAR</v>
       </c>
+      <c r="M1" t="str">
+        <v>HISTORY</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -507,16 +510,19 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K3">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L3">
         <v>2025</v>
+      </c>
+      <c r="M3" t="str">
+        <v>2025-07-19_2025-07-24</v>
       </c>
     </row>
     <row r="4">
@@ -545,16 +551,19 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K4">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L4">
         <v>2025</v>
+      </c>
+      <c r="M4" t="str">
+        <v>2025-07-19_2025-07-24</v>
       </c>
     </row>
     <row r="5">
@@ -583,16 +592,19 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J5">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K5">
         <v>31</v>
       </c>
       <c r="L5">
         <v>2025</v>
+      </c>
+      <c r="M5" t="str">
+        <v>2025-07-19_2025-07-24</v>
       </c>
     </row>
     <row r="6">
@@ -624,13 +636,16 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K6">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="L6">
         <v>2025</v>
+      </c>
+      <c r="M6" t="str">
+        <v>2025-07-21_2025-07-27</v>
       </c>
     </row>
     <row r="7">
@@ -662,13 +677,16 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K7">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="L7">
         <v>2025</v>
+      </c>
+      <c r="M7" t="str">
+        <v>2025-07-21_2025-07-27</v>
       </c>
     </row>
     <row r="8">
@@ -700,13 +718,16 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K8">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="L8">
         <v>2025</v>
+      </c>
+      <c r="M8" t="str">
+        <v>2025-07-21_2025-07-27</v>
       </c>
     </row>
     <row r="9">
@@ -776,13 +797,16 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K10">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="L10">
         <v>2025</v>
+      </c>
+      <c r="M10" t="str">
+        <v>2025-07-25_2025-07-28</v>
       </c>
     </row>
     <row r="11">
@@ -814,13 +838,16 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>2025</v>
+      </c>
+      <c r="M11" t="str">
+        <v>2025-08-01_2025-08-31</v>
       </c>
     </row>
     <row r="12">
@@ -7171,7 +7198,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L178"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M178"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix app add new pagination features
</commit_message>
<xml_diff>
--- a/data/db/employes.xlsx
+++ b/data/db/employes.xlsx
@@ -3,11 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="employes" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">employes!$A$2:$L$165</definedName>
-  </definedNames>
 </workbook>
 </file>
 
@@ -400,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M178"/>
+  <dimension ref="A1:M193"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -475,10 +472,10 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <v>2025</v>
@@ -510,19 +507,16 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>2025</v>
-      </c>
-      <c r="M3" t="str">
-        <v>2025-07-19_2025-07-24</v>
       </c>
     </row>
     <row r="4">
@@ -551,19 +545,16 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <v>2025</v>
-      </c>
-      <c r="M4" t="str">
-        <v>2025-07-19_2025-07-24</v>
       </c>
     </row>
     <row r="5">
@@ -592,19 +583,16 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <v>2025</v>
-      </c>
-      <c r="M5" t="str">
-        <v>2025-07-19_2025-07-24</v>
       </c>
     </row>
     <row r="6">
@@ -636,16 +624,13 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <v>2025</v>
-      </c>
-      <c r="M6" t="str">
-        <v>2025-07-21_2025-07-27</v>
       </c>
     </row>
     <row r="7">
@@ -677,16 +662,13 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>2025</v>
-      </c>
-      <c r="M7" t="str">
-        <v>2025-07-21_2025-07-27</v>
       </c>
     </row>
     <row r="8">
@@ -718,16 +700,13 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <v>2025</v>
-      </c>
-      <c r="M8" t="str">
-        <v>2025-07-21_2025-07-27</v>
       </c>
     </row>
     <row r="9">
@@ -759,10 +738,10 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <v>2025</v>
@@ -797,16 +776,13 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>2025</v>
-      </c>
-      <c r="M10" t="str">
-        <v>2025-07-25_2025-07-28</v>
       </c>
     </row>
     <row r="11">
@@ -846,9 +822,6 @@
       <c r="L11">
         <v>2025</v>
       </c>
-      <c r="M11" t="str">
-        <v>2025-08-01_2025-08-31</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -879,10 +852,10 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>2025</v>
@@ -917,10 +890,10 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>2025</v>
@@ -955,10 +928,10 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <v>2025</v>
@@ -993,10 +966,10 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <v>2025</v>
@@ -1031,10 +1004,10 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>2025</v>
@@ -1069,10 +1042,10 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <v>2025</v>
@@ -1107,10 +1080,10 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>2025</v>
@@ -1145,10 +1118,10 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L19">
         <v>2025</v>
@@ -1183,10 +1156,10 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L20">
         <v>2025</v>
@@ -1221,10 +1194,10 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K21">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <v>2025</v>
@@ -1259,10 +1232,10 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K22">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L22">
         <v>2025</v>
@@ -1297,10 +1270,10 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K23">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <v>2025</v>
@@ -1335,10 +1308,10 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K24">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>2025</v>
@@ -1373,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K25">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L25">
         <v>2025</v>
@@ -1411,10 +1384,10 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K26">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L26">
         <v>2025</v>
@@ -1449,10 +1422,10 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K27">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L27">
         <v>2025</v>
@@ -1487,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L28">
         <v>2025</v>
@@ -1525,10 +1498,10 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K29">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L29">
         <v>2025</v>
@@ -1563,10 +1536,10 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K30">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L30">
         <v>2025</v>
@@ -1601,10 +1574,10 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K31">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L31">
         <v>2025</v>
@@ -1639,10 +1612,10 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K32">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L32">
         <v>2025</v>
@@ -1677,10 +1650,10 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K33">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L33">
         <v>2025</v>
@@ -1715,10 +1688,10 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K34">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L34">
         <v>2025</v>
@@ -1753,10 +1726,10 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K35">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L35">
         <v>2025</v>
@@ -1791,10 +1764,10 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K36">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L36">
         <v>2025</v>
@@ -1829,10 +1802,10 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K37">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L37">
         <v>2025</v>
@@ -1867,10 +1840,10 @@
         <v>0</v>
       </c>
       <c r="J38">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K38">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L38">
         <v>2025</v>
@@ -1905,10 +1878,10 @@
         <v>0</v>
       </c>
       <c r="J39">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K39">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L39">
         <v>2025</v>
@@ -1943,10 +1916,10 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K40">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L40">
         <v>2025</v>
@@ -1981,10 +1954,10 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K41">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L41">
         <v>2025</v>
@@ -2019,10 +1992,10 @@
         <v>0</v>
       </c>
       <c r="J42">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K42">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L42">
         <v>2025</v>
@@ -2057,10 +2030,10 @@
         <v>0</v>
       </c>
       <c r="J43">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K43">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L43">
         <v>2025</v>
@@ -2095,10 +2068,10 @@
         <v>0</v>
       </c>
       <c r="J44">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K44">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L44">
         <v>2025</v>
@@ -2133,10 +2106,10 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K45">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L45">
         <v>2025</v>
@@ -2171,10 +2144,10 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K46">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L46">
         <v>2025</v>
@@ -2209,10 +2182,10 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K47">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L47">
         <v>2025</v>
@@ -2247,10 +2220,10 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K48">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L48">
         <v>2025</v>
@@ -2285,10 +2258,10 @@
         <v>0</v>
       </c>
       <c r="J49">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K49">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L49">
         <v>2025</v>
@@ -2323,10 +2296,10 @@
         <v>0</v>
       </c>
       <c r="J50">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K50">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L50">
         <v>2025</v>
@@ -2361,10 +2334,10 @@
         <v>0</v>
       </c>
       <c r="J51">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K51">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L51">
         <v>2025</v>
@@ -2399,10 +2372,10 @@
         <v>0</v>
       </c>
       <c r="J52">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K52">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L52">
         <v>2025</v>
@@ -2437,10 +2410,10 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K53">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L53">
         <v>2025</v>
@@ -2475,10 +2448,10 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K54">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L54">
         <v>2025</v>
@@ -2513,10 +2486,10 @@
         <v>0</v>
       </c>
       <c r="J55">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K55">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L55">
         <v>2025</v>
@@ -2551,10 +2524,10 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K56">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L56">
         <v>2025</v>
@@ -2589,10 +2562,10 @@
         <v>0</v>
       </c>
       <c r="J57">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K57">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L57">
         <v>2025</v>
@@ -2627,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="J58">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K58">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L58">
         <v>2025</v>
@@ -2665,10 +2638,10 @@
         <v>0</v>
       </c>
       <c r="J59">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K59">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L59">
         <v>2025</v>
@@ -2703,10 +2676,10 @@
         <v>0</v>
       </c>
       <c r="J60">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K60">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L60">
         <v>2025</v>
@@ -2741,10 +2714,10 @@
         <v>0</v>
       </c>
       <c r="J61">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K61">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L61">
         <v>2025</v>
@@ -2779,10 +2752,10 @@
         <v>0</v>
       </c>
       <c r="J62">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K62">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L62">
         <v>2025</v>
@@ -2817,10 +2790,10 @@
         <v>0</v>
       </c>
       <c r="J63">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K63">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L63">
         <v>2025</v>
@@ -2855,10 +2828,10 @@
         <v>0</v>
       </c>
       <c r="J64">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K64">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L64">
         <v>2025</v>
@@ -2893,10 +2866,10 @@
         <v>0</v>
       </c>
       <c r="J65">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K65">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L65">
         <v>2025</v>
@@ -2931,10 +2904,10 @@
         <v>0</v>
       </c>
       <c r="J66">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K66">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L66">
         <v>2025</v>
@@ -2969,10 +2942,10 @@
         <v>0</v>
       </c>
       <c r="J67">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K67">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L67">
         <v>2025</v>
@@ -3007,10 +2980,10 @@
         <v>0</v>
       </c>
       <c r="J68">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K68">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L68">
         <v>2025</v>
@@ -3045,10 +3018,10 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K69">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L69">
         <v>2025</v>
@@ -3083,10 +3056,10 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K70">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L70">
         <v>2025</v>
@@ -3121,10 +3094,10 @@
         <v>0</v>
       </c>
       <c r="J71">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K71">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L71">
         <v>2025</v>
@@ -3159,10 +3132,10 @@
         <v>0</v>
       </c>
       <c r="J72">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K72">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L72">
         <v>2025</v>
@@ -3197,10 +3170,10 @@
         <v>0</v>
       </c>
       <c r="J73">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K73">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L73">
         <v>2025</v>
@@ -3235,10 +3208,10 @@
         <v>0</v>
       </c>
       <c r="J74">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K74">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L74">
         <v>2025</v>
@@ -3273,10 +3246,10 @@
         <v>0</v>
       </c>
       <c r="J75">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K75">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L75">
         <v>2025</v>
@@ -3311,10 +3284,10 @@
         <v>0</v>
       </c>
       <c r="J76">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K76">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L76">
         <v>2025</v>
@@ -3349,10 +3322,10 @@
         <v>0</v>
       </c>
       <c r="J77">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K77">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L77">
         <v>2025</v>
@@ -3387,10 +3360,10 @@
         <v>0</v>
       </c>
       <c r="J78">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K78">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L78">
         <v>2025</v>
@@ -3425,10 +3398,10 @@
         <v>0</v>
       </c>
       <c r="J79">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K79">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L79">
         <v>2025</v>
@@ -3463,10 +3436,10 @@
         <v>0</v>
       </c>
       <c r="J80">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K80">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L80">
         <v>2025</v>
@@ -3501,10 +3474,10 @@
         <v>0</v>
       </c>
       <c r="J81">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K81">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L81">
         <v>2025</v>
@@ -3539,10 +3512,10 @@
         <v>0</v>
       </c>
       <c r="J82">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K82">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L82">
         <v>2025</v>
@@ -3577,10 +3550,10 @@
         <v>0</v>
       </c>
       <c r="J83">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K83">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L83">
         <v>2025</v>
@@ -3615,10 +3588,10 @@
         <v>0</v>
       </c>
       <c r="J84">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K84">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L84">
         <v>2025</v>
@@ -3653,10 +3626,10 @@
         <v>0</v>
       </c>
       <c r="J85">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K85">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L85">
         <v>2025</v>
@@ -3691,10 +3664,10 @@
         <v>0</v>
       </c>
       <c r="J86">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K86">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L86">
         <v>2025</v>
@@ -3729,10 +3702,10 @@
         <v>0</v>
       </c>
       <c r="J87">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K87">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L87">
         <v>2025</v>
@@ -3767,10 +3740,10 @@
         <v>0</v>
       </c>
       <c r="J88">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K88">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L88">
         <v>2025</v>
@@ -3805,10 +3778,10 @@
         <v>0</v>
       </c>
       <c r="J89">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K89">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L89">
         <v>2025</v>
@@ -3843,10 +3816,10 @@
         <v>0</v>
       </c>
       <c r="J90">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K90">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L90">
         <v>2025</v>
@@ -3881,10 +3854,10 @@
         <v>0</v>
       </c>
       <c r="J91">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K91">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L91">
         <v>2025</v>
@@ -3919,10 +3892,10 @@
         <v>0</v>
       </c>
       <c r="J92">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K92">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L92">
         <v>2025</v>
@@ -3957,10 +3930,10 @@
         <v>0</v>
       </c>
       <c r="J93">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K93">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L93">
         <v>2025</v>
@@ -3995,10 +3968,10 @@
         <v>0</v>
       </c>
       <c r="J94">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K94">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L94">
         <v>2025</v>
@@ -4033,10 +4006,10 @@
         <v>0</v>
       </c>
       <c r="J95">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K95">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L95">
         <v>2025</v>
@@ -4071,10 +4044,10 @@
         <v>0</v>
       </c>
       <c r="J96">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K96">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L96">
         <v>2025</v>
@@ -4109,10 +4082,10 @@
         <v>0</v>
       </c>
       <c r="J97">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K97">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L97">
         <v>2025</v>
@@ -4147,10 +4120,10 @@
         <v>0</v>
       </c>
       <c r="J98">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K98">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L98">
         <v>2025</v>
@@ -4185,10 +4158,10 @@
         <v>0</v>
       </c>
       <c r="J99">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K99">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L99">
         <v>2025</v>
@@ -4223,10 +4196,10 @@
         <v>0</v>
       </c>
       <c r="J100">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K100">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L100">
         <v>2025</v>
@@ -4261,10 +4234,10 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K101">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L101">
         <v>2025</v>
@@ -4299,10 +4272,10 @@
         <v>0</v>
       </c>
       <c r="J102">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K102">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L102">
         <v>2025</v>
@@ -4337,10 +4310,10 @@
         <v>0</v>
       </c>
       <c r="J103">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K103">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L103">
         <v>2025</v>
@@ -4375,10 +4348,10 @@
         <v>0</v>
       </c>
       <c r="J104">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K104">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L104">
         <v>2025</v>
@@ -4413,10 +4386,10 @@
         <v>0</v>
       </c>
       <c r="J105">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K105">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L105">
         <v>2025</v>
@@ -4451,10 +4424,10 @@
         <v>0</v>
       </c>
       <c r="J106">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K106">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L106">
         <v>2025</v>
@@ -4489,10 +4462,10 @@
         <v>0</v>
       </c>
       <c r="J107">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K107">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L107">
         <v>2025</v>
@@ -4527,10 +4500,10 @@
         <v>0</v>
       </c>
       <c r="J108">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K108">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L108">
         <v>2025</v>
@@ -4565,10 +4538,10 @@
         <v>0</v>
       </c>
       <c r="J109">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K109">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L109">
         <v>2025</v>
@@ -4603,10 +4576,10 @@
         <v>0</v>
       </c>
       <c r="J110">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K110">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L110">
         <v>2025</v>
@@ -4641,10 +4614,10 @@
         <v>0</v>
       </c>
       <c r="J111">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K111">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L111">
         <v>2025</v>
@@ -4679,10 +4652,10 @@
         <v>0</v>
       </c>
       <c r="J112">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K112">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L112">
         <v>2025</v>
@@ -4717,10 +4690,10 @@
         <v>0</v>
       </c>
       <c r="J113">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K113">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L113">
         <v>2025</v>
@@ -4755,10 +4728,10 @@
         <v>0</v>
       </c>
       <c r="J114">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K114">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L114">
         <v>2025</v>
@@ -4793,10 +4766,10 @@
         <v>0</v>
       </c>
       <c r="J115">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K115">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L115">
         <v>2025</v>
@@ -4831,10 +4804,10 @@
         <v>0</v>
       </c>
       <c r="J116">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K116">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L116">
         <v>2025</v>
@@ -4869,10 +4842,10 @@
         <v>0</v>
       </c>
       <c r="J117">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K117">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L117">
         <v>2025</v>
@@ -4907,10 +4880,10 @@
         <v>0</v>
       </c>
       <c r="J118">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K118">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L118">
         <v>2025</v>
@@ -4945,10 +4918,10 @@
         <v>0</v>
       </c>
       <c r="J119">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K119">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L119">
         <v>2025</v>
@@ -4983,10 +4956,10 @@
         <v>0</v>
       </c>
       <c r="J120">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K120">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L120">
         <v>2025</v>
@@ -5021,10 +4994,10 @@
         <v>0</v>
       </c>
       <c r="J121">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K121">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L121">
         <v>2025</v>
@@ -5059,10 +5032,10 @@
         <v>0</v>
       </c>
       <c r="J122">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K122">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L122">
         <v>2025</v>
@@ -5097,10 +5070,10 @@
         <v>0</v>
       </c>
       <c r="J123">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K123">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L123">
         <v>2025</v>
@@ -5135,10 +5108,10 @@
         <v>0</v>
       </c>
       <c r="J124">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K124">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L124">
         <v>2025</v>
@@ -5173,10 +5146,10 @@
         <v>0</v>
       </c>
       <c r="J125">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K125">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L125">
         <v>2025</v>
@@ -5211,10 +5184,10 @@
         <v>0</v>
       </c>
       <c r="J126">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K126">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L126">
         <v>2025</v>
@@ -5249,10 +5222,10 @@
         <v>0</v>
       </c>
       <c r="J127">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K127">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L127">
         <v>2025</v>
@@ -5287,10 +5260,10 @@
         <v>0</v>
       </c>
       <c r="J128">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K128">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L128">
         <v>2025</v>
@@ -5325,10 +5298,10 @@
         <v>0</v>
       </c>
       <c r="J129">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K129">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L129">
         <v>2025</v>
@@ -5363,10 +5336,10 @@
         <v>0</v>
       </c>
       <c r="J130">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K130">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L130">
         <v>2025</v>
@@ -5401,10 +5374,10 @@
         <v>0</v>
       </c>
       <c r="J131">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K131">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L131">
         <v>2025</v>
@@ -5439,10 +5412,10 @@
         <v>0</v>
       </c>
       <c r="J132">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K132">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L132">
         <v>2025</v>
@@ -5477,10 +5450,10 @@
         <v>0</v>
       </c>
       <c r="J133">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K133">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L133">
         <v>2025</v>
@@ -5515,10 +5488,10 @@
         <v>0</v>
       </c>
       <c r="J134">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K134">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L134">
         <v>2025</v>
@@ -5553,10 +5526,10 @@
         <v>0</v>
       </c>
       <c r="J135">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K135">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L135">
         <v>2025</v>
@@ -5591,10 +5564,10 @@
         <v>0</v>
       </c>
       <c r="J136">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K136">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L136">
         <v>2025</v>
@@ -5629,10 +5602,10 @@
         <v>0</v>
       </c>
       <c r="J137">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K137">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L137">
         <v>2025</v>
@@ -5667,10 +5640,10 @@
         <v>0</v>
       </c>
       <c r="J138">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K138">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L138">
         <v>2025</v>
@@ -5705,10 +5678,10 @@
         <v>0</v>
       </c>
       <c r="J139">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K139">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L139">
         <v>2025</v>
@@ -5743,10 +5716,10 @@
         <v>0</v>
       </c>
       <c r="J140">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K140">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L140">
         <v>2025</v>
@@ -5781,10 +5754,10 @@
         <v>0</v>
       </c>
       <c r="J141">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K141">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L141">
         <v>2025</v>
@@ -5819,10 +5792,10 @@
         <v>0</v>
       </c>
       <c r="J142">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K142">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L142">
         <v>2025</v>
@@ -5857,10 +5830,10 @@
         <v>0</v>
       </c>
       <c r="J143">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K143">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L143">
         <v>2025</v>
@@ -5895,10 +5868,10 @@
         <v>0</v>
       </c>
       <c r="J144">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K144">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L144">
         <v>2025</v>
@@ -5933,10 +5906,10 @@
         <v>0</v>
       </c>
       <c r="J145">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K145">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L145">
         <v>2025</v>
@@ -5971,10 +5944,10 @@
         <v>0</v>
       </c>
       <c r="J146">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K146">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L146">
         <v>2025</v>
@@ -6009,10 +5982,10 @@
         <v>0</v>
       </c>
       <c r="J147">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K147">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L147">
         <v>2025</v>
@@ -6047,10 +6020,10 @@
         <v>0</v>
       </c>
       <c r="J148">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K148">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L148">
         <v>2025</v>
@@ -6085,10 +6058,10 @@
         <v>0</v>
       </c>
       <c r="J149">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K149">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L149">
         <v>2025</v>
@@ -6123,10 +6096,10 @@
         <v>0</v>
       </c>
       <c r="J150">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K150">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L150">
         <v>2025</v>
@@ -6161,10 +6134,10 @@
         <v>0</v>
       </c>
       <c r="J151">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K151">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L151">
         <v>2025</v>
@@ -6199,10 +6172,10 @@
         <v>0</v>
       </c>
       <c r="J152">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K152">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L152">
         <v>2025</v>
@@ -6237,10 +6210,10 @@
         <v>0</v>
       </c>
       <c r="J153">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K153">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L153">
         <v>2025</v>
@@ -6275,10 +6248,10 @@
         <v>0</v>
       </c>
       <c r="J154">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K154">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L154">
         <v>2025</v>
@@ -6313,10 +6286,10 @@
         <v>0</v>
       </c>
       <c r="J155">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K155">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L155">
         <v>2025</v>
@@ -6351,10 +6324,10 @@
         <v>0</v>
       </c>
       <c r="J156">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K156">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L156">
         <v>2025</v>
@@ -6389,10 +6362,10 @@
         <v>0</v>
       </c>
       <c r="J157">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K157">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L157">
         <v>2025</v>
@@ -6427,10 +6400,10 @@
         <v>0</v>
       </c>
       <c r="J158">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K158">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L158">
         <v>2025</v>
@@ -6465,10 +6438,10 @@
         <v>0</v>
       </c>
       <c r="J159">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K159">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L159">
         <v>2025</v>
@@ -6503,10 +6476,10 @@
         <v>0</v>
       </c>
       <c r="J160">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K160">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L160">
         <v>2025</v>
@@ -6541,10 +6514,10 @@
         <v>0</v>
       </c>
       <c r="J161">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K161">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L161">
         <v>2025</v>
@@ -6579,10 +6552,10 @@
         <v>0</v>
       </c>
       <c r="J162">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K162">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L162">
         <v>2025</v>
@@ -6617,10 +6590,10 @@
         <v>0</v>
       </c>
       <c r="J163">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K163">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L163">
         <v>2025</v>
@@ -6655,10 +6628,10 @@
         <v>0</v>
       </c>
       <c r="J164">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K164">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L164">
         <v>2025</v>
@@ -6693,10 +6666,10 @@
         <v>0</v>
       </c>
       <c r="J165">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K165">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L165">
         <v>2025</v>
@@ -6731,10 +6704,10 @@
         <v>0</v>
       </c>
       <c r="J166">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K166">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L166">
         <v>2025</v>
@@ -6769,10 +6742,10 @@
         <v>0</v>
       </c>
       <c r="J167">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K167">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L167">
         <v>2025</v>
@@ -6807,10 +6780,10 @@
         <v>0</v>
       </c>
       <c r="J168">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K168">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L168">
         <v>2025</v>
@@ -6845,10 +6818,10 @@
         <v>0</v>
       </c>
       <c r="J169">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K169">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L169">
         <v>2025</v>
@@ -6883,10 +6856,10 @@
         <v>0</v>
       </c>
       <c r="J170">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K170">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L170">
         <v>2025</v>
@@ -6921,10 +6894,10 @@
         <v>0</v>
       </c>
       <c r="J171">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K171">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L171">
         <v>2025</v>
@@ -6959,10 +6932,10 @@
         <v>0</v>
       </c>
       <c r="J172">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K172">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L172">
         <v>2025</v>
@@ -6997,10 +6970,10 @@
         <v>0</v>
       </c>
       <c r="J173">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K173">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L173">
         <v>2025</v>
@@ -7035,10 +7008,10 @@
         <v>0</v>
       </c>
       <c r="J174">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K174">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L174">
         <v>2025</v>
@@ -7073,10 +7046,10 @@
         <v>0</v>
       </c>
       <c r="J175">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K175">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L175">
         <v>2025</v>
@@ -7111,10 +7084,10 @@
         <v>0</v>
       </c>
       <c r="J176">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K176">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L176">
         <v>2025</v>
@@ -7149,10 +7122,10 @@
         <v>0</v>
       </c>
       <c r="J177">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K177">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L177">
         <v>2025</v>
@@ -7187,18 +7160,603 @@
         <v>0</v>
       </c>
       <c r="J178">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K178">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="L178">
         <v>2025</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="str">
+        <v>525</v>
+      </c>
+      <c r="B179" t="str">
+        <v>424</v>
+      </c>
+      <c r="C179" t="str">
+        <v>424242</v>
+      </c>
+      <c r="D179" t="str">
+        <v>2242</v>
+      </c>
+      <c r="E179" t="str">
+        <v>4242</v>
+      </c>
+      <c r="F179" t="str">
+        <v>4242</v>
+      </c>
+      <c r="G179" t="str">
+        <v>4242</v>
+      </c>
+      <c r="H179">
+        <v>0</v>
+      </c>
+      <c r="I179">
+        <v>0</v>
+      </c>
+      <c r="J179">
+        <v>22</v>
+      </c>
+      <c r="K179">
+        <v>22</v>
+      </c>
+      <c r="L179">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>1111</v>
+      </c>
+      <c r="B180" t="str">
+        <v>1111</v>
+      </c>
+      <c r="C180" t="str">
+        <v>1111</v>
+      </c>
+      <c r="D180" t="str">
+        <v>1111</v>
+      </c>
+      <c r="E180" t="str">
+        <v>1111</v>
+      </c>
+      <c r="F180" t="str">
+        <v>1111</v>
+      </c>
+      <c r="G180" t="str">
+        <v>1111</v>
+      </c>
+      <c r="H180">
+        <v>0</v>
+      </c>
+      <c r="I180">
+        <v>0</v>
+      </c>
+      <c r="J180">
+        <v>1111</v>
+      </c>
+      <c r="K180">
+        <v>1111</v>
+      </c>
+      <c r="L180">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="str">
+        <v>1123</v>
+      </c>
+      <c r="B181" t="str">
+        <v>1123</v>
+      </c>
+      <c r="C181" t="str">
+        <v>1123</v>
+      </c>
+      <c r="D181" t="str">
+        <v>1123</v>
+      </c>
+      <c r="E181" t="str">
+        <v>1123</v>
+      </c>
+      <c r="F181" t="str">
+        <v>1123</v>
+      </c>
+      <c r="G181" t="str">
+        <v>1123</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+      <c r="I181">
+        <v>0</v>
+      </c>
+      <c r="J181">
+        <v>1123</v>
+      </c>
+      <c r="K181">
+        <v>1123</v>
+      </c>
+      <c r="L181">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="str">
+        <v>4141</v>
+      </c>
+      <c r="B182" t="str">
+        <v>4141</v>
+      </c>
+      <c r="C182" t="str">
+        <v>4141</v>
+      </c>
+      <c r="D182" t="str">
+        <v>4141</v>
+      </c>
+      <c r="E182" t="str">
+        <v>4141</v>
+      </c>
+      <c r="F182" t="str">
+        <v>4141</v>
+      </c>
+      <c r="G182" t="str">
+        <v>4141</v>
+      </c>
+      <c r="H182">
+        <v>0</v>
+      </c>
+      <c r="I182">
+        <v>0</v>
+      </c>
+      <c r="J182">
+        <v>4141</v>
+      </c>
+      <c r="K182">
+        <v>4141</v>
+      </c>
+      <c r="L182">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="str">
+        <v>4141</v>
+      </c>
+      <c r="B183" t="str">
+        <v>4141</v>
+      </c>
+      <c r="C183" t="str">
+        <v>4141</v>
+      </c>
+      <c r="D183" t="str">
+        <v>4141</v>
+      </c>
+      <c r="E183" t="str">
+        <v>4141</v>
+      </c>
+      <c r="F183" t="str">
+        <v>4141</v>
+      </c>
+      <c r="G183" t="str">
+        <v>4141</v>
+      </c>
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183">
+        <v>0</v>
+      </c>
+      <c r="J183">
+        <v>4141</v>
+      </c>
+      <c r="K183">
+        <v>4141</v>
+      </c>
+      <c r="L183">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="str">
+        <v>4141</v>
+      </c>
+      <c r="B184" t="str">
+        <v>4141</v>
+      </c>
+      <c r="C184" t="str">
+        <v>4141</v>
+      </c>
+      <c r="D184" t="str">
+        <v>4141</v>
+      </c>
+      <c r="E184" t="str">
+        <v>4141</v>
+      </c>
+      <c r="F184" t="str">
+        <v>4141</v>
+      </c>
+      <c r="G184" t="str">
+        <v>4141</v>
+      </c>
+      <c r="H184">
+        <v>0</v>
+      </c>
+      <c r="I184">
+        <v>0</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="K184">
+        <v>0</v>
+      </c>
+      <c r="L184">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="str">
+        <v>757852</v>
+      </c>
+      <c r="B185" t="str">
+        <v>757852</v>
+      </c>
+      <c r="C185" t="str">
+        <v>757852</v>
+      </c>
+      <c r="D185" t="str">
+        <v>757852</v>
+      </c>
+      <c r="E185" t="str">
+        <v>757852</v>
+      </c>
+      <c r="F185" t="str">
+        <v>757852</v>
+      </c>
+      <c r="G185" t="str">
+        <v>757852</v>
+      </c>
+      <c r="H185">
+        <v>0</v>
+      </c>
+      <c r="I185">
+        <v>0</v>
+      </c>
+      <c r="J185">
+        <v>0</v>
+      </c>
+      <c r="K185">
+        <v>0</v>
+      </c>
+      <c r="L185">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="str">
+        <v>b452542</v>
+      </c>
+      <c r="B186" t="str">
+        <v>245245</v>
+      </c>
+      <c r="C186" t="str">
+        <v>254254245</v>
+      </c>
+      <c r="D186" t="str">
+        <v>2542542</v>
+      </c>
+      <c r="E186" t="str">
+        <v>254245</v>
+      </c>
+      <c r="F186" t="str">
+        <v>54254254</v>
+      </c>
+      <c r="G186" t="str">
+        <v>2542452</v>
+      </c>
+      <c r="H186">
+        <v>0</v>
+      </c>
+      <c r="I186">
+        <v>0</v>
+      </c>
+      <c r="J186">
+        <v>2452</v>
+      </c>
+      <c r="K186">
+        <v>2452</v>
+      </c>
+      <c r="L186">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="str">
+        <v>25572</v>
+      </c>
+      <c r="B187" t="str">
+        <v>872872872</v>
+      </c>
+      <c r="C187" t="str">
+        <v>27272</v>
+      </c>
+      <c r="D187" t="str">
+        <v>782782</v>
+      </c>
+      <c r="E187" t="str">
+        <v>78272</v>
+      </c>
+      <c r="F187" t="str">
+        <v>78272</v>
+      </c>
+      <c r="G187" t="str">
+        <v>87287278</v>
+      </c>
+      <c r="H187">
+        <v>0</v>
+      </c>
+      <c r="I187">
+        <v>0</v>
+      </c>
+      <c r="J187">
+        <v>0</v>
+      </c>
+      <c r="K187">
+        <v>0</v>
+      </c>
+      <c r="L187">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="str">
+        <v>2583543</v>
+      </c>
+      <c r="B188" t="str">
+        <v>34563</v>
+      </c>
+      <c r="C188" t="str">
+        <v>435643546</v>
+      </c>
+      <c r="D188" t="str">
+        <v>56356345</v>
+      </c>
+      <c r="E188" t="str">
+        <v>6534563</v>
+      </c>
+      <c r="F188" t="str">
+        <v>635643563</v>
+      </c>
+      <c r="G188" t="str">
+        <v>56435643</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+      <c r="I188">
+        <v>0</v>
+      </c>
+      <c r="J188">
+        <v>1407</v>
+      </c>
+      <c r="K188">
+        <v>1407</v>
+      </c>
+      <c r="L188">
+        <v>2025</v>
+      </c>
+      <c r="M188" t="str">
+        <v>2025-07-21_2025-07-27</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="str">
+        <v>42452</v>
+      </c>
+      <c r="B189" t="str">
+        <v>452452</v>
+      </c>
+      <c r="C189" t="str">
+        <v>452542</v>
+      </c>
+      <c r="D189" t="str">
+        <v>24524</v>
+      </c>
+      <c r="E189" t="str">
+        <v>2542</v>
+      </c>
+      <c r="F189" t="str">
+        <v>245245</v>
+      </c>
+      <c r="G189" t="str">
+        <v>24245</v>
+      </c>
+      <c r="H189">
+        <v>0</v>
+      </c>
+      <c r="I189">
+        <v>0</v>
+      </c>
+      <c r="J189">
+        <v>0</v>
+      </c>
+      <c r="K189">
+        <v>0</v>
+      </c>
+      <c r="L189">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="str">
+        <v>47174</v>
+      </c>
+      <c r="B190" t="str">
+        <v>47174</v>
+      </c>
+      <c r="C190" t="str">
+        <v>47174</v>
+      </c>
+      <c r="D190" t="str">
+        <v>47174</v>
+      </c>
+      <c r="E190" t="str">
+        <v>47174</v>
+      </c>
+      <c r="F190" t="str">
+        <v>47174</v>
+      </c>
+      <c r="G190" t="str">
+        <v>4717447174</v>
+      </c>
+      <c r="H190">
+        <v>0</v>
+      </c>
+      <c r="I190">
+        <v>0</v>
+      </c>
+      <c r="J190">
+        <v>47143</v>
+      </c>
+      <c r="K190">
+        <v>47143</v>
+      </c>
+      <c r="L190">
+        <v>2025</v>
+      </c>
+      <c r="M190" t="str">
+        <v>2025-08-01_2025-08-31</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="str">
+        <v>8873</v>
+      </c>
+      <c r="B191" t="str">
+        <v>8873</v>
+      </c>
+      <c r="C191" t="str">
+        <v>8873</v>
+      </c>
+      <c r="D191" t="str">
+        <v>8873</v>
+      </c>
+      <c r="E191" t="str">
+        <v>8873</v>
+      </c>
+      <c r="F191" t="str">
+        <v>8873</v>
+      </c>
+      <c r="G191" t="str">
+        <v>8873</v>
+      </c>
+      <c r="H191">
+        <v>0</v>
+      </c>
+      <c r="I191">
+        <v>0</v>
+      </c>
+      <c r="J191">
+        <v>4</v>
+      </c>
+      <c r="K191">
+        <v>4</v>
+      </c>
+      <c r="L191">
+        <v>2025</v>
+      </c>
+      <c r="M191" t="str">
+        <v>2025-07-21_2025-07-27</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="str">
+        <v>rferf11451</v>
+      </c>
+      <c r="B192" t="str">
+        <v>rferf11451</v>
+      </c>
+      <c r="C192" t="str">
+        <v>rferf11451</v>
+      </c>
+      <c r="D192" t="str">
+        <v>rferf11451</v>
+      </c>
+      <c r="E192" t="str">
+        <v>rferf11451</v>
+      </c>
+      <c r="F192" t="str">
+        <v>rferf11451</v>
+      </c>
+      <c r="G192" t="str">
+        <v>rferf11451</v>
+      </c>
+      <c r="H192">
+        <v>0</v>
+      </c>
+      <c r="I192">
+        <v>0</v>
+      </c>
+      <c r="J192">
+        <v>4</v>
+      </c>
+      <c r="K192">
+        <v>4</v>
+      </c>
+      <c r="L192">
+        <v>2025</v>
+      </c>
+      <c r="M192" t="str">
+        <v>2025-07-21_2025-07-27</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="str">
+        <v>254725742</v>
+      </c>
+      <c r="B193" t="str">
+        <v>254725742</v>
+      </c>
+      <c r="C193" t="str">
+        <v>254725742</v>
+      </c>
+      <c r="D193" t="str">
+        <v>254725742</v>
+      </c>
+      <c r="E193" t="str">
+        <v>254725742</v>
+      </c>
+      <c r="F193" t="str">
+        <v>254725742</v>
+      </c>
+      <c r="G193" t="str">
+        <v>254725742</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="I193">
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>4</v>
+      </c>
+      <c r="K193">
+        <v>4</v>
+      </c>
+      <c r="L193">
+        <v>2025</v>
+      </c>
+      <c r="M193" t="str">
+        <v>2025-07-21_2025-07-27</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M178"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M193"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>